<commit_message>
Table and question are done for the moment
</commit_message>
<xml_diff>
--- a/evaluation/evaluationResults.xlsx
+++ b/evaluation/evaluationResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="42">
   <si>
     <t>Course</t>
   </si>
@@ -136,13 +136,22 @@
   </si>
   <si>
     <t>Support</t>
+  </si>
+  <si>
+    <t>RCC</t>
+  </si>
+  <si>
+    <t>PT Strålsäkerhet</t>
+  </si>
+  <si>
+    <t>Telia GDPR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +184,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -193,7 +210,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -235,8 +252,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -246,8 +279,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="57">
     <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="6" builtinId="9" hidden="1"/>
@@ -268,6 +305,14 @@
     <cellStyle name="Följd hyperlänk" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
@@ -288,6 +333,14 @@
     <cellStyle name="Hyperlänk" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -617,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -936,6 +989,873 @@
         <v>4</v>
       </c>
     </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>